<commit_message>
modify some intefaces and test success.
</commit_message>
<xml_diff>
--- a/databaseDesign/医疗app系统接口.xlsx
+++ b/databaseDesign/医疗app系统接口.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\medicalApp_Background_System\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\medicalApp_Background_System\databaseDesign\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="23">
   <si>
     <t>接口名称</t>
   </si>
@@ -99,6 +99,26 @@
   </si>
   <si>
     <t>后台提供url，前端提供就诊人ID</t>
+    <phoneticPr fontId="6" type="noConversion"/>
+  </si>
+  <si>
+    <t>Appoitment</t>
+    <phoneticPr fontId="6" type="noConversion"/>
+  </si>
+  <si>
+    <t>注册用户</t>
+    <phoneticPr fontId="6" type="noConversion"/>
+  </si>
+  <si>
+    <t>后台提供url，前端把注册信息传给后台，后台进行校验和数据插入，返回结果给前端</t>
+    <phoneticPr fontId="6" type="noConversion"/>
+  </si>
+  <si>
+    <t>注册页面</t>
+    <phoneticPr fontId="6" type="noConversion"/>
+  </si>
+  <si>
+    <t>客户表customer</t>
     <phoneticPr fontId="6" type="noConversion"/>
   </si>
 </sst>
@@ -540,7 +560,7 @@
   <dimension ref="A1:E39"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="A34" sqref="A34:XFD34"/>
+      <selection activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4"/>
@@ -637,13 +657,26 @@
         <v>17</v>
       </c>
       <c r="D6" s="4"/>
-      <c r="E6" s="9"/>
-    </row>
-    <row r="7" spans="1:5">
-      <c r="B7" s="4"/>
-      <c r="C7" s="5"/>
-      <c r="D7" s="4"/>
-      <c r="E7" s="9"/>
+      <c r="E6" s="4" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" ht="43.2">
+      <c r="A7">
+        <v>6</v>
+      </c>
+      <c r="B7" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="C7" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="D7" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="E7" s="4" t="s">
+        <v>22</v>
+      </c>
     </row>
     <row r="8" spans="1:5">
       <c r="B8" s="4"/>
@@ -788,6 +821,6 @@
   </sheetData>
   <phoneticPr fontId="6" type="noConversion"/>
   <pageMargins left="0.69930555555555596" right="0.69930555555555596" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
database sql update and inteface infomation update
</commit_message>
<xml_diff>
--- a/databaseDesign/医疗app系统接口.xlsx
+++ b/databaseDesign/医疗app系统接口.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="34">
   <si>
     <t>接口名称</t>
   </si>
@@ -110,15 +110,48 @@
     <phoneticPr fontId="6" type="noConversion"/>
   </si>
   <si>
-    <t>后台提供url，前端把注册信息传给后台，后台进行校验和数据插入，返回结果给前端</t>
-    <phoneticPr fontId="6" type="noConversion"/>
-  </si>
-  <si>
     <t>注册页面</t>
     <phoneticPr fontId="6" type="noConversion"/>
   </si>
   <si>
     <t>客户表customer</t>
+    <phoneticPr fontId="6" type="noConversion"/>
+  </si>
+  <si>
+    <t>医院介绍</t>
+  </si>
+  <si>
+    <t>后台提供url，前端获取到医院详细信息和所有科室名字</t>
+  </si>
+  <si>
+    <t>医院表hospital和科室表section</t>
+  </si>
+  <si>
+    <t>医生选择</t>
+  </si>
+  <si>
+    <t>后台提供url，前端提供6中所选的科室名称， 后台根据科室名称返回前端该科室下所有医生列表</t>
+  </si>
+  <si>
+    <t>医生表doctor</t>
+  </si>
+  <si>
+    <t>医生详细信息</t>
+  </si>
+  <si>
+    <t>前端提供7中所选的医生id，后端返回选择医生的所有详细信息</t>
+  </si>
+  <si>
+    <t>医院导航界面</t>
+  </si>
+  <si>
+    <t>后台提供医院交通官方网站交通</t>
+  </si>
+  <si>
+    <t>医院表hospital</t>
+  </si>
+  <si>
+    <t>后台提供url，前端把注册信息传给后台，后台进行校验和数据插入，返回结果给前端（要进行校验！！！）</t>
     <phoneticPr fontId="6" type="noConversion"/>
   </si>
 </sst>
@@ -559,8 +592,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E39"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="A8" sqref="A8"/>
+    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4"/>
@@ -661,7 +694,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="7" spans="1:5" ht="43.2">
+    <row r="7" spans="1:5" ht="57.6">
       <c r="A7">
         <v>6</v>
       </c>
@@ -669,38 +702,74 @@
         <v>19</v>
       </c>
       <c r="C7" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="D7" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="D7" s="4" t="s">
+      <c r="E7" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="E7" s="4" t="s">
+    </row>
+    <row r="8" spans="1:5" ht="28.8">
+      <c r="A8">
+        <v>7</v>
+      </c>
+      <c r="B8" s="4" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="8" spans="1:5">
-      <c r="B8" s="4"/>
-      <c r="C8" s="5"/>
+      <c r="C8" s="5" t="s">
+        <v>23</v>
+      </c>
       <c r="D8" s="4"/>
-      <c r="E8" s="9"/>
-    </row>
-    <row r="9" spans="1:5">
-      <c r="B9" s="4"/>
-      <c r="C9" s="5"/>
+      <c r="E8" s="9" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" ht="43.2">
+      <c r="A9">
+        <v>8</v>
+      </c>
+      <c r="B9" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="C9" s="5" t="s">
+        <v>26</v>
+      </c>
       <c r="D9" s="4"/>
-      <c r="E9" s="9"/>
-    </row>
-    <row r="10" spans="1:5">
-      <c r="B10" s="4"/>
-      <c r="C10" s="5"/>
+      <c r="E9" s="9" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" ht="28.8">
+      <c r="A10">
+        <v>9</v>
+      </c>
+      <c r="B10" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="C10" s="5" t="s">
+        <v>29</v>
+      </c>
       <c r="D10" s="4"/>
-      <c r="E10" s="9"/>
+      <c r="E10" s="9" t="s">
+        <v>27</v>
+      </c>
     </row>
     <row r="11" spans="1:5">
-      <c r="B11" s="4"/>
-      <c r="C11" s="5"/>
+      <c r="A11">
+        <v>10</v>
+      </c>
+      <c r="B11" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="C11" s="5" t="s">
+        <v>31</v>
+      </c>
       <c r="D11" s="4"/>
-      <c r="E11" s="9"/>
+      <c r="E11" s="9" t="s">
+        <v>32</v>
+      </c>
     </row>
     <row r="12" spans="1:5">
       <c r="B12" s="6"/>

</xml_diff>

<commit_message>
intefaces modify in excel
</commit_message>
<xml_diff>
--- a/databaseDesign/医疗app系统接口.xlsx
+++ b/databaseDesign/医疗app系统接口.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="51">
   <si>
     <t>接口名称</t>
   </si>
@@ -82,10 +82,6 @@
     <phoneticPr fontId="6" type="noConversion"/>
   </si>
   <si>
-    <t>门诊表</t>
-    <phoneticPr fontId="6" type="noConversion"/>
-  </si>
-  <si>
     <t>周排班表</t>
     <phoneticPr fontId="6" type="noConversion"/>
   </si>
@@ -152,6 +148,115 @@
   </si>
   <si>
     <t>后台提供url，前端把注册信息传给后台，后台进行校验和数据插入，返回结果给前端（要进行校验！！！）</t>
+    <phoneticPr fontId="6" type="noConversion"/>
+  </si>
+  <si>
+    <t>特色科室</t>
+    <phoneticPr fontId="6" type="noConversion"/>
+  </si>
+  <si>
+    <t>前台查询，后台返回所有的特色科室名称</t>
+    <phoneticPr fontId="6" type="noConversion"/>
+  </si>
+  <si>
+    <t>特色科室界面</t>
+    <phoneticPr fontId="6" type="noConversion"/>
+  </si>
+  <si>
+    <t>门诊表outpatient</t>
+    <phoneticPr fontId="6" type="noConversion"/>
+  </si>
+  <si>
+    <t>科室详细信息查询</t>
+    <phoneticPr fontId="6" type="noConversion"/>
+  </si>
+  <si>
+    <t>前台传给后台科室id信息，后台根据科室id进行记录的查询</t>
+    <phoneticPr fontId="6" type="noConversion"/>
+  </si>
+  <si>
+    <t>科室介绍界面</t>
+    <phoneticPr fontId="6" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t>U</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>RL</t>
+    </r>
+    <phoneticPr fontId="6" type="noConversion"/>
+  </si>
+  <si>
+    <t>192.168.1.134:8080/framework/customer/loginVerifyByUserName</t>
+    <phoneticPr fontId="6" type="noConversion"/>
+  </si>
+  <si>
+    <t>192.168.1.134:8080/framework/section/selectAllSection</t>
+  </si>
+  <si>
+    <t>192.168.1.134:8080/framework/section/selectAllSection</t>
+    <phoneticPr fontId="6" type="noConversion"/>
+  </si>
+  <si>
+    <t>192.168.1.134:8080/framework/outpatient/selectByExample</t>
+    <phoneticPr fontId="6" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t>192.168.1.134:8080/framework/customer/</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>register</t>
+    </r>
+    <phoneticPr fontId="6" type="noConversion"/>
+  </si>
+  <si>
+    <t>192.168.1.134:8080/framework/hospital/searchHosInfo</t>
+  </si>
+  <si>
+    <t>192.168.1.134:8080/framework/hospital/searchHosInfo</t>
+    <phoneticPr fontId="6" type="noConversion"/>
+  </si>
+  <si>
+    <t>192.168.1.134:8080/framework/doctor/selectBySection</t>
+    <phoneticPr fontId="6" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t>192.168.1.134:8080/framework/doctor/</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>searchDoctorInfo</t>
+    </r>
+    <phoneticPr fontId="6" type="noConversion"/>
+  </si>
+  <si>
+    <t>192.168.1.134:8080/framework/section/searchSectionInfo</t>
     <phoneticPr fontId="6" type="noConversion"/>
   </si>
 </sst>
@@ -232,7 +337,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -252,6 +357,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="常规" xfId="0" builtinId="0"/>
@@ -590,22 +698,23 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E39"/>
+  <dimension ref="A1:F39"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+    <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="F13" sqref="F13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4"/>
   <cols>
     <col min="1" max="1" width="9" customWidth="1"/>
-    <col min="2" max="2" width="22.109375" customWidth="1"/>
-    <col min="3" max="3" width="31.33203125" style="1" customWidth="1"/>
-    <col min="4" max="4" width="21.6640625" customWidth="1"/>
-    <col min="5" max="5" width="12.6640625" customWidth="1"/>
+    <col min="2" max="2" width="20.33203125" customWidth="1"/>
+    <col min="3" max="3" width="33.109375" style="1" customWidth="1"/>
+    <col min="4" max="4" width="22.5546875" customWidth="1"/>
+    <col min="5" max="5" width="29.33203125" customWidth="1"/>
+    <col min="6" max="6" width="53.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5">
+    <row r="1" spans="1:6">
       <c r="B1" t="s">
         <v>0</v>
       </c>
@@ -618,8 +727,11 @@
       <c r="E1" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="2" spans="1:5" ht="57.6">
+      <c r="F1" s="4" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" ht="57.6">
       <c r="A2">
         <v>1</v>
       </c>
@@ -635,8 +747,11 @@
       <c r="E2" s="4" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="3" spans="1:5" ht="57.6">
+      <c r="F2" s="4" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" ht="43.2">
       <c r="A3">
         <v>2</v>
       </c>
@@ -650,8 +765,11 @@
       <c r="E3" s="4" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="4" spans="1:5" ht="72">
+      <c r="F3" s="4" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" ht="72">
       <c r="A4">
         <v>3</v>
       </c>
@@ -663,135 +781,183 @@
       </c>
       <c r="D4" s="4"/>
       <c r="E4" s="4" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5">
+        <v>36</v>
+      </c>
+      <c r="F4" s="4" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6">
       <c r="A5">
         <v>4</v>
       </c>
       <c r="B5" s="4" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C5" s="5"/>
       <c r="D5" s="4" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="E5" s="9"/>
     </row>
-    <row r="6" spans="1:5">
+    <row r="6" spans="1:6">
       <c r="A6">
         <v>5</v>
       </c>
       <c r="B6" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="C6" s="5" t="s">
         <v>16</v>
-      </c>
-      <c r="C6" s="5" t="s">
-        <v>17</v>
       </c>
       <c r="D6" s="4"/>
       <c r="E6" s="4" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" ht="57.6">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" ht="43.2">
       <c r="A7">
         <v>6</v>
       </c>
       <c r="B7" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="C7" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="D7" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="C7" s="5" t="s">
-        <v>33</v>
-      </c>
-      <c r="D7" s="4" t="s">
+      <c r="E7" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="E7" s="4" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" ht="28.8">
+      <c r="F7" s="4" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" ht="28.8">
       <c r="A8">
         <v>7</v>
       </c>
       <c r="B8" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="C8" s="5" t="s">
         <v>22</v>
-      </c>
-      <c r="C8" s="5" t="s">
-        <v>23</v>
       </c>
       <c r="D8" s="4"/>
       <c r="E8" s="9" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" ht="43.2">
+        <v>23</v>
+      </c>
+      <c r="F8" s="4" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" ht="43.2">
       <c r="A9">
         <v>8</v>
       </c>
       <c r="B9" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="C9" s="5" t="s">
         <v>25</v>
-      </c>
-      <c r="C9" s="5" t="s">
-        <v>26</v>
       </c>
       <c r="D9" s="4"/>
       <c r="E9" s="9" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5" ht="28.8">
+        <v>26</v>
+      </c>
+      <c r="F9" s="4" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" ht="28.8">
       <c r="A10">
         <v>9</v>
       </c>
       <c r="B10" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="C10" s="5" t="s">
         <v>28</v>
-      </c>
-      <c r="C10" s="5" t="s">
-        <v>29</v>
       </c>
       <c r="D10" s="4"/>
       <c r="E10" s="9" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5">
+        <v>26</v>
+      </c>
+      <c r="F10" s="4" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6">
       <c r="A11">
         <v>10</v>
       </c>
       <c r="B11" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="C11" s="5" t="s">
         <v>30</v>
-      </c>
-      <c r="C11" s="5" t="s">
-        <v>31</v>
       </c>
       <c r="D11" s="4"/>
       <c r="E11" s="9" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5">
-      <c r="B12" s="6"/>
-      <c r="C12" s="7"/>
-      <c r="D12" s="8"/>
-    </row>
-    <row r="13" spans="1:5">
-      <c r="B13" s="6"/>
-      <c r="C13" s="7"/>
-      <c r="D13" s="8"/>
-    </row>
-    <row r="14" spans="1:5">
+        <v>31</v>
+      </c>
+      <c r="F11" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" ht="28.8">
+      <c r="A12">
+        <v>11</v>
+      </c>
+      <c r="B12" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="C12" s="11" t="s">
+        <v>34</v>
+      </c>
+      <c r="D12" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="E12" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="F12" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" ht="28.8">
+      <c r="A13">
+        <v>12</v>
+      </c>
+      <c r="B13" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="C13" s="11" t="s">
+        <v>38</v>
+      </c>
+      <c r="D13" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="E13" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="F13" s="4" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6">
       <c r="B14" s="6"/>
       <c r="D14" s="8"/>
     </row>
-    <row r="15" spans="1:5">
+    <row r="15" spans="1:6">
       <c r="B15" s="6"/>
       <c r="C15" s="7"/>
       <c r="D15" s="8"/>
       <c r="E15" s="9"/>
     </row>
-    <row r="16" spans="1:5">
+    <row r="16" spans="1:6">
       <c r="B16" s="6"/>
       <c r="C16" s="7"/>
       <c r="D16" s="8"/>

</xml_diff>